<commit_message>
added windows io support
</commit_message>
<xml_diff>
--- a/课程设计要求/课程设计实验报告模板(2023秋).xlsx
+++ b/课程设计要求/课程设计实验报告模板(2023秋).xlsx
@@ -3,7 +3,7 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="24701"/>
   <workbookPr filterPrivacy="1"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4198CE13-B621-4EB1-AB43-1BC431FFB26B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3B980A36-63D0-4AC3-B812-2383E6C9E4BE}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="30936" windowHeight="16896" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="19" uniqueCount="19">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="23" uniqueCount="23">
   <si>
     <t>小组成员</t>
   </si>
@@ -71,9 +71,6 @@
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
-    <t>Brainfuck jit解释器</t>
-  </si>
-  <si>
     <t>叶恒迪</t>
   </si>
   <si>
@@ -84,6 +81,35 @@
   </si>
   <si>
     <t>编写代码和编写报告和编写ppt</t>
+  </si>
+  <si>
+    <t>Brainf**k jit解释器</t>
+  </si>
+  <si>
+    <t xml:space="preserve">首先将程序解析为指令流, 然后做简单的折叠优化, 变成IR流, 在IR流上渐进的执行一系列窥孔优化, 使其变快, 然后利用pypeach库将得到的IR转化为机器代码, 并跳转过去执行, 以达到jit的效果. </t>
+  </si>
+  <si>
+    <t>使用visualize.py作为主程序, 其接受一些参数并作出对应的可视化展示, 在命令行模式下, 程序启动后立马开始运行, 运行结束即退出, 在图形模式下, 程序会接受用户的按键, 单步或连续运行, 并逐步展示虚拟机内部的状态. 使用方法见help文本:
+usage: visualize.py [-h] [-o OPTIMIZE] [-i INPUT] [-f FILE] [-g GRAPHIC] [-j JIT] [-r IR]
+brainfuck visualizer
+optional arguments:
+  -h, --help            show this help message and exit
+  -o OPTIMIZE, --optimize OPTIMIZE
+                        turn on to enable optimize, note that only if ir was enabled will this option make sense
+  -i INPUT, --input INPUT
+                        input to the program
+  -f FILE, --file FILE  bf program
+  -g GRAPHIC, --graphic GRAPHIC
+                        turn on to enable visualize
+  -j JIT, --jit JIT     turn on to enable jit(NOT compatible with graphic), with this on, you CANNOT pass input by argument, please use a pipe
+  -r IR, --ir IR        turn on to enable ir</t>
+  </si>
+  <si>
+    <t>命令行模式下运行截图:
+可视化模式下运行截图:</t>
+  </si>
+  <si>
+    <t>写晕过去了</t>
   </si>
 </sst>
 </file>
@@ -136,7 +162,7 @@
       <patternFill patternType="gray125"/>
     </fill>
   </fills>
-  <borders count="12">
+  <borders count="15">
     <border>
       <left/>
       <right/>
@@ -299,6 +325,43 @@
         <color indexed="64"/>
       </top>
       <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thick">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top style="thick">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thick">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="thick">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thick">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="thick">
+        <color indexed="64"/>
+      </right>
+      <top style="thick">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thick">
         <color indexed="64"/>
       </bottom>
       <diagonal/>
@@ -308,7 +371,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="19">
+  <cellXfs count="26">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="justify" vertical="center" wrapText="1"/>
@@ -340,6 +403,9 @@
     <xf numFmtId="0" fontId="3" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="justify" vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="10" xfId="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="justify" vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -361,8 +427,26 @@
     <xf numFmtId="0" fontId="3" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="10" xfId="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="justify" vertical="center" wrapText="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="justify" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="justify" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="justify" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="justify" vertical="top" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="2">
@@ -380,6 +464,161 @@
     </ext>
   </extLst>
 </styleSheet>
+</file>
+
+<file path=xl/drawings/drawing1.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>1</xdr:col>
+      <xdr:colOff>22860</xdr:colOff>
+      <xdr:row>9</xdr:row>
+      <xdr:rowOff>294792</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>5</xdr:col>
+      <xdr:colOff>1630680</xdr:colOff>
+      <xdr:row>9</xdr:row>
+      <xdr:rowOff>784911</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="7" name="图片 6">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{AAD5D449-9C55-4FE9-9F88-4FB57D8C4850}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId1">
+          <a:extLst>
+            <a:ext uri="{28A0092B-C50C-407E-A947-70E740481C1C}">
+              <a14:useLocalDpi xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" val="0"/>
+            </a:ext>
+          </a:extLst>
+        </a:blip>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="990600" y="4836312"/>
+          <a:ext cx="6126480" cy="490119"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>4</xdr:col>
+      <xdr:colOff>960119</xdr:colOff>
+      <xdr:row>9</xdr:row>
+      <xdr:rowOff>1211698</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>5</xdr:col>
+      <xdr:colOff>3310968</xdr:colOff>
+      <xdr:row>9</xdr:row>
+      <xdr:rowOff>3360419</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="9" name="图片 8">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{6A326AB9-C2B4-46C9-B2BF-35E558C19E4B}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId2" cstate="print">
+          <a:extLst>
+            <a:ext uri="{28A0092B-C50C-407E-A947-70E740481C1C}">
+              <a14:useLocalDpi xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" val="0"/>
+            </a:ext>
+          </a:extLst>
+        </a:blip>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="5128259" y="10157578"/>
+          <a:ext cx="3669109" cy="2148721"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>1</xdr:col>
+      <xdr:colOff>76200</xdr:colOff>
+      <xdr:row>9</xdr:row>
+      <xdr:rowOff>1176184</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>4</xdr:col>
+      <xdr:colOff>594360</xdr:colOff>
+      <xdr:row>9</xdr:row>
+      <xdr:rowOff>3359473</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="11" name="图片 10">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{DE24E7CC-9131-4E0C-88CE-F4D9E0FC5FF9}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId3" cstate="print">
+          <a:extLst>
+            <a:ext uri="{28A0092B-C50C-407E-A947-70E740481C1C}">
+              <a14:useLocalDpi xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" val="0"/>
+            </a:ext>
+          </a:extLst>
+        </a:blip>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="1043940" y="10122064"/>
+          <a:ext cx="3718560" cy="2183289"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+</xdr:wsDr>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -647,8 +886,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:F12"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="I6" sqref="I6"/>
+    <sheetView tabSelected="1" topLeftCell="A10" workbookViewId="0">
+      <selection activeCell="P10" sqref="P10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4"/>
@@ -658,40 +897,40 @@
     <col min="3" max="3" width="19" customWidth="1"/>
     <col min="4" max="4" width="18.21875" customWidth="1"/>
     <col min="5" max="5" width="19.21875" customWidth="1"/>
-    <col min="6" max="6" width="30.77734375" customWidth="1"/>
+    <col min="6" max="6" width="50.88671875" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:6" ht="37.200000000000003" thickBot="1">
-      <c r="A1" s="11" t="s">
+      <c r="A1" s="12" t="s">
         <v>7</v>
       </c>
-      <c r="B1" s="11"/>
-      <c r="C1" s="11"/>
-      <c r="D1" s="11"/>
-      <c r="E1" s="11"/>
-      <c r="F1" s="11"/>
+      <c r="B1" s="12"/>
+      <c r="C1" s="12"/>
+      <c r="D1" s="12"/>
+      <c r="E1" s="12"/>
+      <c r="F1" s="12"/>
     </row>
     <row r="2" spans="1:6" ht="18" thickTop="1">
       <c r="A2" s="1" t="s">
         <v>8</v>
       </c>
-      <c r="B2" s="13" t="s">
-        <v>14</v>
-      </c>
-      <c r="C2" s="13"/>
-      <c r="D2" s="13"/>
-      <c r="E2" s="13"/>
-      <c r="F2" s="14"/>
+      <c r="B2" s="14" t="s">
+        <v>18</v>
+      </c>
+      <c r="C2" s="14"/>
+      <c r="D2" s="14"/>
+      <c r="E2" s="14"/>
+      <c r="F2" s="15"/>
     </row>
     <row r="3" spans="1:6" ht="18" thickBot="1">
-      <c r="A3" s="15" t="s">
+      <c r="A3" s="16" t="s">
         <v>0</v>
       </c>
-      <c r="B3" s="16"/>
-      <c r="C3" s="16"/>
-      <c r="D3" s="16"/>
-      <c r="E3" s="16"/>
-      <c r="F3" s="17"/>
+      <c r="B3" s="17"/>
+      <c r="C3" s="17"/>
+      <c r="D3" s="17"/>
+      <c r="E3" s="17"/>
+      <c r="F3" s="18"/>
     </row>
     <row r="4" spans="1:6" ht="18" thickTop="1">
       <c r="A4" s="1" t="s">
@@ -718,19 +957,19 @@
         <v>201220195</v>
       </c>
       <c r="B5" s="5" t="s">
+        <v>14</v>
+      </c>
+      <c r="C5" s="5" t="s">
         <v>15</v>
-      </c>
-      <c r="C5" s="5" t="s">
-        <v>16</v>
       </c>
       <c r="D5" s="5">
         <v>18071128014</v>
       </c>
-      <c r="E5" s="18" t="s">
+      <c r="E5" s="11" t="s">
+        <v>16</v>
+      </c>
+      <c r="F5" s="6" t="s">
         <v>17</v>
-      </c>
-      <c r="F5" s="6" t="s">
-        <v>18</v>
       </c>
     </row>
     <row r="6" spans="1:6" ht="18" thickBot="1">
@@ -741,55 +980,63 @@
       <c r="E6" s="8"/>
       <c r="F6" s="9"/>
     </row>
-    <row r="7" spans="1:6" ht="50.1" customHeight="1" thickTop="1" thickBot="1">
+    <row r="7" spans="1:6" ht="75.599999999999994" customHeight="1" thickTop="1" thickBot="1">
       <c r="A7" s="10" t="s">
         <v>10</v>
       </c>
-      <c r="B7" s="12"/>
-      <c r="C7" s="12"/>
-      <c r="D7" s="12"/>
-      <c r="E7" s="12"/>
-      <c r="F7" s="12"/>
+      <c r="B7" s="22" t="s">
+        <v>19</v>
+      </c>
+      <c r="C7" s="23"/>
+      <c r="D7" s="23"/>
+      <c r="E7" s="23"/>
+      <c r="F7" s="24"/>
     </row>
     <row r="8" spans="1:6" ht="75.75" customHeight="1" thickTop="1" thickBot="1">
       <c r="A8" s="10" t="s">
         <v>11</v>
       </c>
-      <c r="B8" s="12"/>
-      <c r="C8" s="12"/>
-      <c r="D8" s="12"/>
-      <c r="E8" s="12"/>
-      <c r="F8" s="12"/>
+      <c r="B8" s="13"/>
+      <c r="C8" s="13"/>
+      <c r="D8" s="13"/>
+      <c r="E8" s="13"/>
+      <c r="F8" s="13"/>
     </row>
-    <row r="9" spans="1:6" ht="115.5" customHeight="1" thickTop="1" thickBot="1">
+    <row r="9" spans="1:6" ht="409.2" customHeight="1" thickTop="1" thickBot="1">
       <c r="A9" s="10" t="s">
         <v>12</v>
       </c>
-      <c r="B9" s="12"/>
-      <c r="C9" s="12"/>
-      <c r="D9" s="12"/>
-      <c r="E9" s="12"/>
-      <c r="F9" s="12"/>
+      <c r="B9" s="19" t="s">
+        <v>20</v>
+      </c>
+      <c r="C9" s="20"/>
+      <c r="D9" s="20"/>
+      <c r="E9" s="20"/>
+      <c r="F9" s="21"/>
     </row>
-    <row r="10" spans="1:6" ht="139.94999999999999" customHeight="1" thickTop="1" thickBot="1">
+    <row r="10" spans="1:6" ht="409.2" customHeight="1" thickTop="1" thickBot="1">
       <c r="A10" s="10" t="s">
         <v>13</v>
       </c>
-      <c r="B10" s="12"/>
-      <c r="C10" s="12"/>
-      <c r="D10" s="12"/>
-      <c r="E10" s="12"/>
-      <c r="F10" s="12"/>
+      <c r="B10" s="25" t="s">
+        <v>21</v>
+      </c>
+      <c r="C10" s="25"/>
+      <c r="D10" s="25"/>
+      <c r="E10" s="25"/>
+      <c r="F10" s="25"/>
     </row>
     <row r="11" spans="1:6" ht="50.1" customHeight="1" thickTop="1" thickBot="1">
       <c r="A11" s="10" t="s">
         <v>6</v>
       </c>
-      <c r="B11" s="12"/>
-      <c r="C11" s="12"/>
-      <c r="D11" s="12"/>
-      <c r="E11" s="12"/>
-      <c r="F11" s="12"/>
+      <c r="B11" s="13" t="s">
+        <v>22</v>
+      </c>
+      <c r="C11" s="13"/>
+      <c r="D11" s="13"/>
+      <c r="E11" s="13"/>
+      <c r="F11" s="13"/>
     </row>
     <row r="12" spans="1:6" ht="15" thickTop="1"/>
   </sheetData>
@@ -809,5 +1056,6 @@
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId2"/>
+  <drawing r:id="rId3"/>
 </worksheet>
 </file>
</xml_diff>